<commit_message>
cleaned up and merged login tests for both partner and insder apps
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20354"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RoshikaG\UPN New\UPN_Insider_App\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arshadm\Documents\Growth project automation\UPN_New_Login\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642BE519-69F6-4C32-B5D0-BF70D776C9B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7106BF-BA12-470D-ACED-1964D3CB14DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25140" windowHeight="10960" tabRatio="911" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10957" tabRatio="911" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="changeName_happyPath" sheetId="9" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="nullPassword_Login" sheetId="85" r:id="rId9"/>
     <sheet name="validation_Login" sheetId="86" r:id="rId10"/>
     <sheet name="successfully_Login" sheetId="87" r:id="rId11"/>
+    <sheet name="setUp" sheetId="88" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="55">
   <si>
     <t>Y</t>
   </si>
@@ -191,6 +192,15 @@
   </si>
   <si>
     <t>ROSHIKAG@99X.LK</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://partner.qa.upnorway.net/</t>
+  </si>
+  <si>
+    <t>https://insider.qa.upnorway.net/</t>
   </si>
 </sst>
 </file>
@@ -522,17 +532,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -549,7 +559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -566,7 +576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -583,7 +593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -600,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -640,14 +650,14 @@
       <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.26953125" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" customWidth="1"/>
-    <col min="3" max="3" width="52.453125" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="52.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -661,7 +671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -675,7 +685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
@@ -708,13 +718,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -728,7 +738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -742,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
@@ -756,7 +766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -783,6 +793,39 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9AC076-49A2-45DE-8A5C-4E0EC75B51FA}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{B5CAB901-7AFC-48F1-A7F3-97B67233826F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E313AB86-FBAC-47C9-BF52-892C7B013052}">
   <dimension ref="A1:E5"/>
@@ -791,9 +834,9 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -810,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -821,7 +864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -838,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -855,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -886,17 +929,17 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.453125" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" customWidth="1"/>
-    <col min="6" max="6" width="45.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="45.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -919,7 +962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -942,7 +985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -965,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -988,7 +1031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1039,17 +1082,17 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="53.36328125" customWidth="1"/>
+    <col min="6" max="6" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1072,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -1115,13 +1158,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="52.6328125" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1132,7 +1175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -1143,7 +1186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -1167,13 +1210,13 @@
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1"/>
-    <col min="2" max="2" width="45.1796875" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="45.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1184,7 +1227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1211,15 +1254,15 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" customWidth="1"/>
-    <col min="5" max="5" width="44.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="44.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1239,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -1257,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -1298,14 +1341,14 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" customWidth="1"/>
-    <col min="3" max="3" width="59.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="59.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1319,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
@@ -1346,13 +1389,13 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
-    <col min="3" max="3" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1366,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>

</xml_diff>